<commit_message>
Update template and applied bulk insert
</commit_message>
<xml_diff>
--- a/public/templates/template_enrollment.xlsx
+++ b/public/templates/template_enrollment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loyol\Documents\My Web Applications\convo-analysis\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loyol\Documents\Projects\Conversational Analysis\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0259F76-6637-4081-8D72-34CC9B0A8BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2116A1-8746-4E37-8800-FD7DA6F30FAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3DE51BE9-E12A-4405-A3EC-E03036B025C7}"/>
   </bookViews>
@@ -25,43 +25,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>HEI NAME</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The yellow </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cell</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is pertaining to the existing academic year, this can be more than one.</t>
-    </r>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>2017-F</t>
+  </si>
+  <si>
+    <t>2017-M</t>
+  </si>
+  <si>
+    <t>HEI Code</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Major</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,12 +70,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -123,16 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,61 +429,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A289815C-5811-4FDE-BEA4-92821BBEEF7D}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:L5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="D1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="E1" s="3">
-        <v>2019</v>
-      </c>
-      <c r="F1" s="3">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I3" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I3:L5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>